<commit_message>
playerUnion strategy - intermediate
mostly functional - only the write at the end has some trouble (when fixedFileGroup is active)
</commit_message>
<xml_diff>
--- a/PlayersTCDietlikonWinter2018.xlsx
+++ b/PlayersTCDietlikonWinter2018.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sascha\eclipse-workspace\MATSim\tcDietlikon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A63921-4051-4180-836B-E9124BC25CE8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44D0AAC-323F-4B4D-8FAE-80CE949F4580}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1422,7 +1422,7 @@
   <dimension ref="A1:G576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>